<commit_message>
Correct expected clean time index of test case number 7.
</commit_message>
<xml_diff>
--- a/tests/strategies/clean/expected/test_case7.xlsx
+++ b/tests/strategies/clean/expected/test_case7.xlsx
@@ -368,13 +368,13 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -685,8 +685,8 @@
   </sheetPr>
   <dimension ref="A1:AS76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AM1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="10.85" x14ac:dyDescent="0.2"/>
@@ -910,47 +910,47 @@
     </row>
     <row r="5" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
-      <c r="Y5" s="55"/>
-      <c r="Z5" s="55"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="55"/>
-      <c r="AF5" s="55"/>
-      <c r="AG5" s="55"/>
-      <c r="AH5" s="55"/>
-      <c r="AI5" s="55"/>
-      <c r="AJ5" s="55"/>
-      <c r="AK5" s="55"/>
-      <c r="AL5" s="55"/>
-      <c r="AM5" s="55"/>
-      <c r="AN5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="56"/>
+      <c r="AB5" s="56"/>
+      <c r="AC5" s="56"/>
+      <c r="AD5" s="56"/>
+      <c r="AE5" s="56"/>
+      <c r="AF5" s="56"/>
+      <c r="AG5" s="56"/>
+      <c r="AH5" s="56"/>
+      <c r="AI5" s="56"/>
+      <c r="AJ5" s="56"/>
+      <c r="AK5" s="56"/>
+      <c r="AL5" s="56"/>
+      <c r="AM5" s="56"/>
+      <c r="AN5" s="56"/>
       <c r="AO5" s="39"/>
       <c r="AP5" s="39"/>
       <c r="AQ5" s="50"/>
@@ -958,113 +958,113 @@
     </row>
     <row r="6" spans="1:45" s="3" customFormat="1" ht="13.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <v>33604</v>
       </c>
       <c r="C6" s="36"/>
-      <c r="D6" s="56">
-        <f>DATE(YEAR(B6),1,1)</f>
-        <v>33604</v>
+      <c r="D6" s="54">
+        <f>DATE(YEAR(B6)+1,1,1)</f>
+        <v>33970</v>
       </c>
       <c r="E6" s="42"/>
-      <c r="F6" s="56">
-        <f t="shared" ref="F6" si="0">DATE(YEAR(D6),1,1)</f>
-        <v>33604</v>
+      <c r="F6" s="54">
+        <f t="shared" ref="F6" si="0">DATE(YEAR(D6)+1,1,1)</f>
+        <v>34335</v>
       </c>
       <c r="G6" s="42"/>
-      <c r="H6" s="56">
-        <f t="shared" ref="H6" si="1">DATE(YEAR(F6),1,1)</f>
-        <v>33604</v>
+      <c r="H6" s="54">
+        <f t="shared" ref="H6" si="1">DATE(YEAR(F6)+1,1,1)</f>
+        <v>34700</v>
       </c>
       <c r="I6" s="42"/>
-      <c r="J6" s="56">
-        <f t="shared" ref="J6" si="2">DATE(YEAR(H6),1,1)</f>
-        <v>33604</v>
+      <c r="J6" s="54">
+        <f t="shared" ref="J6" si="2">DATE(YEAR(H6)+1,1,1)</f>
+        <v>35065</v>
       </c>
       <c r="K6" s="42"/>
-      <c r="L6" s="56">
-        <f t="shared" ref="L6" si="3">DATE(YEAR(J6),1,1)</f>
-        <v>33604</v>
+      <c r="L6" s="54">
+        <f t="shared" ref="L6" si="3">DATE(YEAR(J6)+1,1,1)</f>
+        <v>35431</v>
       </c>
       <c r="M6" s="42"/>
-      <c r="N6" s="56">
-        <f t="shared" ref="N6" si="4">DATE(YEAR(L6),1,1)</f>
-        <v>33604</v>
+      <c r="N6" s="54">
+        <f t="shared" ref="N6" si="4">DATE(YEAR(L6)+1,1,1)</f>
+        <v>35796</v>
       </c>
       <c r="O6" s="42"/>
-      <c r="P6" s="56">
-        <f t="shared" ref="P6" si="5">DATE(YEAR(N6),1,1)</f>
-        <v>33604</v>
+      <c r="P6" s="54">
+        <f t="shared" ref="P6" si="5">DATE(YEAR(N6)+1,1,1)</f>
+        <v>36161</v>
       </c>
       <c r="Q6" s="42"/>
-      <c r="R6" s="56">
-        <f t="shared" ref="R6" si="6">DATE(YEAR(P6),1,1)</f>
-        <v>33604</v>
+      <c r="R6" s="54">
+        <f t="shared" ref="R6" si="6">DATE(YEAR(P6)+1,1,1)</f>
+        <v>36526</v>
       </c>
       <c r="S6" s="42"/>
-      <c r="T6" s="56">
-        <f t="shared" ref="T6" si="7">DATE(YEAR(R6),1,1)</f>
-        <v>33604</v>
+      <c r="T6" s="54">
+        <f t="shared" ref="T6" si="7">DATE(YEAR(R6)+1,1,1)</f>
+        <v>36892</v>
       </c>
       <c r="U6" s="42"/>
-      <c r="V6" s="56">
-        <f t="shared" ref="V6" si="8">DATE(YEAR(T6),1,1)</f>
-        <v>33604</v>
+      <c r="V6" s="54">
+        <f t="shared" ref="V6" si="8">DATE(YEAR(T6)+1,1,1)</f>
+        <v>37257</v>
       </c>
       <c r="W6" s="42"/>
-      <c r="X6" s="56">
-        <f t="shared" ref="X6" si="9">DATE(YEAR(V6),1,1)</f>
-        <v>33604</v>
+      <c r="X6" s="54">
+        <f t="shared" ref="X6" si="9">DATE(YEAR(V6)+1,1,1)</f>
+        <v>37622</v>
       </c>
       <c r="Y6" s="42"/>
-      <c r="Z6" s="56">
-        <f t="shared" ref="Z6" si="10">DATE(YEAR(X6),1,1)</f>
-        <v>33604</v>
+      <c r="Z6" s="54">
+        <f t="shared" ref="Z6" si="10">DATE(YEAR(X6)+1,1,1)</f>
+        <v>37987</v>
       </c>
       <c r="AA6" s="42"/>
-      <c r="AB6" s="56">
-        <f t="shared" ref="AB6" si="11">DATE(YEAR(Z6),1,1)</f>
-        <v>33604</v>
+      <c r="AB6" s="54">
+        <f t="shared" ref="AB6" si="11">DATE(YEAR(Z6)+1,1,1)</f>
+        <v>38353</v>
       </c>
       <c r="AC6" s="42"/>
-      <c r="AD6" s="56">
-        <f t="shared" ref="AD6" si="12">DATE(YEAR(AB6),1,1)</f>
-        <v>33604</v>
+      <c r="AD6" s="54">
+        <f t="shared" ref="AD6" si="12">DATE(YEAR(AB6)+1,1,1)</f>
+        <v>38718</v>
       </c>
       <c r="AE6" s="42"/>
-      <c r="AF6" s="56">
-        <f t="shared" ref="AF6" si="13">DATE(YEAR(AD6),1,1)</f>
-        <v>33604</v>
+      <c r="AF6" s="54">
+        <f t="shared" ref="AF6" si="13">DATE(YEAR(AD6)+1,1,1)</f>
+        <v>39083</v>
       </c>
       <c r="AG6" s="42"/>
-      <c r="AH6" s="56">
-        <f t="shared" ref="AH6" si="14">DATE(YEAR(AF6),1,1)</f>
-        <v>33604</v>
+      <c r="AH6" s="54">
+        <f t="shared" ref="AH6" si="14">DATE(YEAR(AF6)+1,1,1)</f>
+        <v>39448</v>
       </c>
       <c r="AI6" s="42"/>
-      <c r="AJ6" s="56">
-        <f t="shared" ref="AJ6" si="15">DATE(YEAR(AH6),1,1)</f>
-        <v>33604</v>
+      <c r="AJ6" s="54">
+        <f t="shared" ref="AJ6" si="15">DATE(YEAR(AH6)+1,1,1)</f>
+        <v>39814</v>
       </c>
       <c r="AK6" s="42"/>
-      <c r="AL6" s="56">
-        <f t="shared" ref="AL6" si="16">DATE(YEAR(AJ6),1,1)</f>
-        <v>33604</v>
+      <c r="AL6" s="54">
+        <f t="shared" ref="AL6" si="16">DATE(YEAR(AJ6)+1,1,1)</f>
+        <v>40179</v>
       </c>
       <c r="AM6" s="42"/>
-      <c r="AN6" s="56">
-        <f t="shared" ref="AN6" si="17">DATE(YEAR(AL6),1,1)</f>
-        <v>33604</v>
+      <c r="AN6" s="54">
+        <f t="shared" ref="AN6" si="17">DATE(YEAR(AL6)+1,1,1)</f>
+        <v>40544</v>
       </c>
       <c r="AO6" s="42"/>
-      <c r="AP6" s="56">
-        <f t="shared" ref="AP6" si="18">DATE(YEAR(AN6),1,1)</f>
-        <v>33604</v>
+      <c r="AP6" s="54">
+        <f t="shared" ref="AP6" si="18">DATE(YEAR(AN6)+1,1,1)</f>
+        <v>40909</v>
       </c>
       <c r="AQ6" s="42"/>
-      <c r="AR6" s="56">
-        <f t="shared" ref="AR6" si="19">DATE(YEAR(AP6),1,1)</f>
-        <v>33604</v>
+      <c r="AR6" s="54">
+        <f t="shared" ref="AR6" si="19">DATE(YEAR(AP6)+1,1,1)</f>
+        <v>41275</v>
       </c>
       <c r="AS6" s="42"/>
     </row>
@@ -4925,12 +4925,12 @@
       <c r="AM57" s="13"/>
     </row>
     <row r="58" spans="1:44" ht="11.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="54"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>

</xml_diff>